<commit_message>
Excel file looks ok
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -6,24 +6,42 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" r:id="rId3" sheetId="1"/>
+    <sheet name="Subtotals By Language" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Subtotals By Language</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Markdown</t>
+  </si>
+  <si>
+    <t>Yaml</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>SBT</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Scala</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -70,14 +88,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -88,7 +112,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,14 +124,129 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="2">
+      <c r="A3" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" t="n" s="2">
+        <v>1237.0</v>
+      </c>
+      <c r="C3" t="n" s="2">
+        <v>-19933.0</v>
+      </c>
+      <c r="D3" t="n" s="2">
+        <v>-18696.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="B4" t="n" s="2">
+        <v>735.0</v>
+      </c>
+      <c r="C4" t="n" s="2">
+        <v>-1272.0</v>
+      </c>
+      <c r="D4" t="n" s="2">
+        <v>-537.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="3">
         <v>3</v>
+      </c>
+      <c r="B5" t="n" s="2">
+        <v>400.0</v>
+      </c>
+      <c r="C5" t="n" s="2">
+        <v>-520.0</v>
+      </c>
+      <c r="D5" t="n" s="2">
+        <v>-120.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n" s="2">
+        <v>36.0</v>
+      </c>
+      <c r="C6" t="n" s="2">
+        <v>-36.0</v>
+      </c>
+      <c r="D6" t="n" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C7" t="n" s="2">
+        <v>-3.0</v>
+      </c>
+      <c r="D7" t="n" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n" s="2">
+        <v>121.0</v>
+      </c>
+      <c r="C8" t="n" s="2">
+        <v>-100.0</v>
+      </c>
+      <c r="D8" t="n" s="2">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n" s="2">
+        <v>102.0</v>
+      </c>
+      <c r="C9" t="n" s="2">
+        <v>-10.0</v>
+      </c>
+      <c r="D9" t="n" s="2">
+        <v>92.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n" s="2">
+        <v>41057.0</v>
+      </c>
+      <c r="C10" t="n" s="2">
+        <v>-36906.0</v>
+      </c>
+      <c r="D10" t="n" s="2">
+        <v>4151.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <f>SUM(B3:B10)</f>
+      </c>
+      <c r="C11" s="4">
+        <f>SUM(C3:C10)</f>
+      </c>
+      <c r="D11" s="4">
+        <f>SUM(D3:D10)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>